<commit_message>
Updated everything to Utility and Interface classes, started with csv import
</commit_message>
<xml_diff>
--- a/Project/Staff_List.xlsx
+++ b/Project/Staff_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\LF work\LF running courses\CX2002\Assignment\2024S1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\2002\2002\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA90EAB1-7387-443D-9C48-A8C1C187A849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CEAE6F-4E4D-448D-B659-F295FC173072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Staff ID</t>
   </si>
@@ -74,6 +74,12 @@
   </si>
   <si>
     <t>Sarah Lee</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>pwd</t>
   </si>
 </sst>
 </file>
@@ -441,19 +447,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.77734375" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" customWidth="1"/>
+    <col min="2" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,16 +467,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -478,16 +487,19 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -495,16 +507,19 @@
         <v>15</v>
       </c>
       <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -512,16 +527,19 @@
         <v>16</v>
       </c>
       <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -529,12 +547,15 @@
         <v>17</v>
       </c>
       <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>13</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>40</v>
       </c>
     </row>

</xml_diff>